<commit_message>
master data user -add, test listener qma
</commit_message>
<xml_diff>
--- a/Data Files/TestData/NexCare/Master Data/Data Customer/dataCustomer - add.xlsx
+++ b/Data Files/TestData/NexCare/Master Data/Data Customer/dataCustomer - add.xlsx
@@ -1185,8 +1185,8 @@
   <sheetPr/>
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>

</xml_diff>